<commit_message>
Inputs/outputs with friends clearer
Made the input csv writer append the friends to the file (they were previously missed). The result also prints the number of friends, the minimum size, maximum size, and average sizes of friendships (excluding singleton friendships).

MainFriendship and Main are updated to print the csv results. MainFriendship provides rounding for the friendship problem.
</commit_message>
<xml_diff>
--- a/app/example_format.xlsx
+++ b/app/example_format.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding Projects\TeamSorting\data\nosave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding Projects\TeamSorting\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{470C103F-91B9-47C4-B275-571396B0BB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A423F7D2-9EEB-448D-93F4-7302DE738BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4487" yWindow="427" windowWidth="18426" windowHeight="13480" xr2:uid="{A9146558-39BB-43CA-A636-1DD2EB36AA8C}"/>
+    <workbookView xWindow="1480" yWindow="2220" windowWidth="19200" windowHeight="11180" xr2:uid="{A9146558-39BB-43CA-A636-1DD2EB36AA8C}"/>
   </bookViews>
   <sheets>
     <sheet name="example_format" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -42,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="66">
   <si>
     <t>Teams</t>
   </si>
@@ -234,6 +247,12 @@
   </si>
   <si>
     <t>Below is a given solution for the problem by using this spreadsheet.</t>
+  </si>
+  <si>
+    <t>Friendships</t>
+  </si>
+  <si>
+    <t>friend1</t>
   </si>
 </sst>
 </file>
@@ -1094,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B16524-6476-4155-8EC2-0D974D54325B}">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1115,6 +1134,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2">
@@ -1129,6 +1151,9 @@
       <c r="D2">
         <v>24</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
@@ -1710,227 +1735,108 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
-        <v>43</v>
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" t="s">
-        <v>48</v>
-      </c>
-      <c r="J43" t="s">
-        <v>49</v>
-      </c>
-      <c r="K43" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44">
-        <f>COUNTIF(B$11:B$35, $A44)</f>
-        <v>8</v>
-      </c>
-      <c r="C44">
-        <f>COUNTIF(C$11:C$35, $A44)</f>
-        <v>6</v>
-      </c>
-      <c r="D44">
-        <f>COUNTIF(D$11:D$35, $A44)</f>
-        <v>6</v>
-      </c>
-      <c r="E44" cm="1">
-        <f t="array" ref="E44">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A44) + ($C$11:$C$35=$A44) + ($D$11:$D$35=$A44)) &gt; 0))</f>
-        <v>7</v>
-      </c>
-      <c r="F44" cm="1">
-        <f t="array" ref="F44">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A44) + ($C$11:$C$35=$A44) + ($D$11:$D$35=$A44)) &gt; 0))</f>
-        <v>6</v>
-      </c>
-      <c r="G44" cm="1">
-        <f t="array" ref="G44">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A44) + ($C$11:$C$35=$A44) + ($D$11:$D$35=$A44)) &gt; 0))</f>
-        <v>7</v>
-      </c>
-      <c r="H44" cm="1">
-        <f t="array" ref="H44">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A44) + ($C$11:$C$35=$A44) + ($D$11:$D$35=$A44)) &gt; 0))</f>
-        <v>4</v>
-      </c>
-      <c r="I44">
-        <f>SUM($E44:$H44)</f>
-        <v>24</v>
-      </c>
-      <c r="J44">
-        <f>$G5</f>
-        <v>6</v>
-      </c>
-      <c r="K44">
-        <f>$I44-$J44</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45">
-        <f>COUNTIF(B$11:B$35, $A45)</f>
-        <v>5</v>
-      </c>
-      <c r="C45">
-        <f>COUNTIF(C$11:C$35, $A45)</f>
-        <v>6</v>
-      </c>
-      <c r="D45">
-        <f>COUNTIF(D$11:D$35, $A45)</f>
-        <v>5</v>
-      </c>
-      <c r="E45" cm="1">
-        <f t="array" ref="E45">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A45) + ($C$11:$C$35=$A45) + ($D$11:$D$35=$A45)) &gt; 0))</f>
-        <v>6</v>
-      </c>
-      <c r="F45" cm="1">
-        <f t="array" ref="F45">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A45) + ($C$11:$C$35=$A45) + ($D$11:$D$35=$A45)) &gt; 0))</f>
-        <v>7</v>
-      </c>
-      <c r="G45" cm="1">
-        <f t="array" ref="G45">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A45) + ($C$11:$C$35=$A45) + ($D$11:$D$35=$A45)) &gt; 0))</f>
-        <v>4</v>
-      </c>
-      <c r="H45" cm="1">
-        <f t="array" ref="H45">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A45) + ($C$11:$C$35=$A45) + ($D$11:$D$35=$A45)) &gt; 0))</f>
-        <v>5</v>
-      </c>
-      <c r="I45">
-        <f t="shared" ref="I45:I47" si="2">SUM($E45:$H45)</f>
-        <v>22</v>
-      </c>
-      <c r="J45">
-        <f t="shared" ref="J45:J47" si="3">$G6</f>
-        <v>5</v>
-      </c>
-      <c r="K45">
-        <f t="shared" ref="K45:K47" si="4">$I45-$J45</f>
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46">
-        <f>COUNTIF(B$11:B$35, $A46)</f>
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
         <v>6</v>
       </c>
-      <c r="C46">
-        <f>COUNTIF(C$11:C$35, $A46)</f>
+      <c r="H46" t="s">
         <v>7</v>
       </c>
-      <c r="D46">
-        <f>COUNTIF(D$11:D$35, $A46)</f>
-        <v>4</v>
-      </c>
-      <c r="E46" cm="1">
-        <f t="array" ref="E46">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A46) + ($C$11:$C$35=$A46) + ($D$11:$D$35=$A46)) &gt; 0))</f>
-        <v>7</v>
-      </c>
-      <c r="F46" cm="1">
-        <f t="array" ref="F46">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A46) + ($C$11:$C$35=$A46) + ($D$11:$D$35=$A46)) &gt; 0))</f>
-        <v>7</v>
-      </c>
-      <c r="G46" cm="1">
-        <f t="array" ref="G46">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A46) + ($C$11:$C$35=$A46) + ($D$11:$D$35=$A46)) &gt; 0))</f>
-        <v>6</v>
-      </c>
-      <c r="H46" cm="1">
-        <f t="array" ref="H46">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A46) + ($C$11:$C$35=$A46) + ($D$11:$D$35=$A46)) &gt; 0))</f>
-        <v>1</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="4"/>
-        <v>16</v>
+      <c r="I46" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B47">
-        <f>COUNTIF(B$11:B$35, $A47)</f>
-        <v>5</v>
+        <f t="shared" ref="B47:D50" si="2">COUNTIF(B$11:B$35, $A47)</f>
+        <v>8</v>
       </c>
       <c r="C47">
-        <f>COUNTIF(C$11:C$35, $A47)</f>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="D47">
-        <f>COUNTIF(D$11:D$35, $A47)</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="E47" cm="1">
         <f t="array" ref="E47">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A47) + ($C$11:$C$35=$A47) + ($D$11:$D$35=$A47)) &gt; 0))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F47" cm="1">
         <f t="array" ref="F47">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A47) + ($C$11:$C$35=$A47) + ($D$11:$D$35=$A47)) &gt; 0))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47" cm="1">
         <f t="array" ref="G47">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A47) + ($C$11:$C$35=$A47) + ($D$11:$D$35=$A47)) &gt; 0))</f>
@@ -1941,202 +1847,304 @@
         <v>4</v>
       </c>
       <c r="I47">
+        <f>SUM($E47:$H47)</f>
+        <v>24</v>
+      </c>
+      <c r="J47">
+        <f>$G5</f>
+        <v>6</v>
+      </c>
+      <c r="K47">
+        <f>$I47-$J47</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
         <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E48" cm="1">
+        <f t="array" ref="E48">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A48) + ($C$11:$C$35=$A48) + ($D$11:$D$35=$A48)) &gt; 0))</f>
+        <v>6</v>
+      </c>
+      <c r="F48" cm="1">
+        <f t="array" ref="F48">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A48) + ($C$11:$C$35=$A48) + ($D$11:$D$35=$A48)) &gt; 0))</f>
+        <v>7</v>
+      </c>
+      <c r="G48" cm="1">
+        <f t="array" ref="G48">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A48) + ($C$11:$C$35=$A48) + ($D$11:$D$35=$A48)) &gt; 0))</f>
+        <v>4</v>
+      </c>
+      <c r="H48" cm="1">
+        <f t="array" ref="H48">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A48) + ($C$11:$C$35=$A48) + ($D$11:$D$35=$A48)) &gt; 0))</f>
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <f t="shared" ref="I48:I50" si="3">SUM($E48:$H48)</f>
+        <v>22</v>
+      </c>
+      <c r="J48">
+        <f>$G6</f>
+        <v>5</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ref="K48:K50" si="4">$I48-$J48</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E49" cm="1">
+        <f t="array" ref="E49">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A49) + ($C$11:$C$35=$A49) + ($D$11:$D$35=$A49)) &gt; 0))</f>
+        <v>7</v>
+      </c>
+      <c r="F49" cm="1">
+        <f t="array" ref="F49">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A49) + ($C$11:$C$35=$A49) + ($D$11:$D$35=$A49)) &gt; 0))</f>
+        <v>7</v>
+      </c>
+      <c r="G49" cm="1">
+        <f t="array" ref="G49">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A49) + ($C$11:$C$35=$A49) + ($D$11:$D$35=$A49)) &gt; 0))</f>
+        <v>6</v>
+      </c>
+      <c r="H49" cm="1">
+        <f t="array" ref="H49">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A49) + ($C$11:$C$35=$A49) + ($D$11:$D$35=$A49)) &gt; 0))</f>
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="J49">
+        <f>$G7</f>
+        <v>5</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E50" cm="1">
+        <f t="array" ref="E50">COUNTA(_xlfn._xlws.FILTER(E$11:E$35, (E$11:E$35="Y") * (($B$11:$B$35=$A50) + ($C$11:$C$35=$A50) + ($D$11:$D$35=$A50)) &gt; 0))</f>
+        <v>6</v>
+      </c>
+      <c r="F50" cm="1">
+        <f t="array" ref="F50">COUNTA(_xlfn._xlws.FILTER(F$11:F$35, (F$11:F$35="Y") * (($B$11:$B$35=$A50) + ($C$11:$C$35=$A50) + ($D$11:$D$35=$A50)) &gt; 0))</f>
+        <v>7</v>
+      </c>
+      <c r="G50" cm="1">
+        <f t="array" ref="G50">COUNTA(_xlfn._xlws.FILTER(G$11:G$35, (G$11:G$35="Y") * (($B$11:$B$35=$A50) + ($C$11:$C$35=$A50) + ($D$11:$D$35=$A50)) &gt; 0))</f>
+        <v>7</v>
+      </c>
+      <c r="H50" cm="1">
+        <f t="array" ref="H50">COUNTA(_xlfn._xlws.FILTER(H$11:H$35, (H$11:H$35="Y") * (($B$11:$B$35=$A50) + ($C$11:$C$35=$A50) + ($D$11:$D$35=$A50)) &gt; 0))</f>
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="J47">
-        <f t="shared" si="3"/>
+      <c r="J50">
+        <f>$G8</f>
         <v>4</v>
       </c>
-      <c r="K47">
+      <c r="K50">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A49" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="E49">
+      <c r="E52">
         <f>COUNTIF(E$11:E$35,"Y")</f>
         <v>9</v>
       </c>
-      <c r="F49">
+      <c r="F52">
         <f>COUNTIF(F$11:F$35,"Y")</f>
         <v>9</v>
       </c>
-      <c r="G49">
+      <c r="G52">
         <f>COUNTIF(G$11:G$35,"Y")</f>
         <v>8</v>
       </c>
-      <c r="H49">
+      <c r="H52">
         <f>COUNTIF(H$11:H$35,"Y")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A50" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="E50">
+      <c r="E53">
         <f>SUM(B$5:B$8)</f>
         <v>6</v>
       </c>
-      <c r="F50">
-        <f t="shared" ref="F50:H50" si="5">SUM(C$5:C$8)</f>
+      <c r="F53">
+        <f t="shared" ref="F53:H53" si="5">SUM(C$5:C$8)</f>
         <v>5</v>
       </c>
-      <c r="G50">
+      <c r="G53">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="H50">
+      <c r="H53">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A51" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="E51">
-        <f>E49-E50</f>
+      <c r="E54">
+        <f>E52-E53</f>
         <v>3</v>
       </c>
-      <c r="F51">
-        <f t="shared" ref="F51:H51" si="6">F49-F50</f>
+      <c r="F54">
+        <f t="shared" ref="F54:H54" si="6">F52-F53</f>
         <v>4</v>
       </c>
-      <c r="G51">
+      <c r="G54">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="H51">
+      <c r="H54">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A53" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B53" t="str">
-        <f>IF(OR(MIN(E51:H51)&lt;0, MIN(K44:K47)&lt;0), "INVALID", "VALID")</f>
+      <c r="B56" t="str">
+        <f>IF(OR(MIN(E54:H54)&lt;0, MIN(K47:K50)&lt;0), "INVALID", "VALID")</f>
         <v>VALID</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A54" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A55" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A57" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A59" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A62" t="s">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C62" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A60" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A61" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" t="s">
-        <v>21</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.5">
@@ -2144,29 +2152,29 @@
         <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -2174,13 +2182,13 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.5">
@@ -2188,10 +2196,10 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.5">
@@ -2199,7 +2207,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -2207,35 +2215,35 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.5">
@@ -2243,10 +2251,10 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.5">
@@ -2254,10 +2262,10 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.5">
@@ -2265,43 +2273,43 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C82" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.5">
@@ -2309,9 +2317,42 @@
         <v>62</v>
       </c>
       <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A84" t="s">
+        <v>62</v>
+      </c>
+      <c r="B84" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A85" t="s">
+        <v>62</v>
+      </c>
+      <c r="B85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+      <c r="B86" t="s">
         <v>33</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C86" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>